<commit_message>
feat: Add smart search tools with overview and detail analysis
</commit_message>
<xml_diff>
--- a/docs/テキスト一覧.xlsx
+++ b/docs/テキスト一覧.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects_workspace\02_access\テキスト\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sem3171\claude-test\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0574610B-27D1-4625-9E06-BB2A075B18AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="5370"/>
+    <workbookView xWindow="-19320" yWindow="1590" windowWidth="19440" windowHeight="13920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$38</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$44</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="171">
   <si>
     <t>コピー元ファイルパス</t>
   </si>
@@ -580,11 +581,23 @@
     </rPh>
     <phoneticPr fontId="2"/>
   </si>
+  <si>
+    <t>\\fsshi01\電源機器製造本部共有\39　部材管理課⇒他部署共有\01     PC工程進捗管理\2020.5月～</t>
+  </si>
+  <si>
+    <t>PC生産_生産管理_20250730.xlsx</t>
+  </si>
+  <si>
+    <t>202506末_仕掛明細表_WBS集約(仕掛年齢付与)_0701.xlsx</t>
+  </si>
+  <si>
+    <t>\\fssha01\全社共有\経営企画部　経理課\情ｼｽ在庫ﾃﾞｰﾀ\仕掛品</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -710,21 +723,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
-    <cellStyle name="標準_Sheet1" xfId="1"/>
+    <cellStyle name="標準_Sheet1" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1001,19 +1014,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G44"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C26" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="76" customWidth="1"/>
+    <col min="1" max="1" width="104.75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="39.25" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.9140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="61.08203125" customWidth="1"/>
@@ -1872,8 +1885,24 @@
         <v>165</v>
       </c>
     </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47" t="s">
+        <v>167</v>
+      </c>
+      <c r="B47" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48" t="s">
+        <v>170</v>
+      </c>
+      <c r="B48" t="s">
+        <v>169</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:G38"/>
+  <autoFilter ref="A1:G44" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>